<commit_message>
feat:add rc block list
</commit_message>
<xml_diff>
--- a/file/柱SCAN.xlsx
+++ b/file/柱SCAN.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\BeamQC\TEST\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\BeamQC\file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9F05B2C-C74E-4B1C-BB98-EE6AAE4E2E25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{849B2A3C-0F7E-4915-BE48-7E73B155FE09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="30" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{8C2A7BE7-2142-4FCC-89B4-3B139FDB86C0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{8C2A7BE7-2142-4FCC-89B4-3B139FDB86C0}"/>
   </bookViews>
   <sheets>
     <sheet name="柱" sheetId="1" r:id="rId1"/>
@@ -1116,57 +1116,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="微軟正黑體"/>
-        <family val="2"/>
-        <charset val="136"/>
-      </rPr>
-      <t>【</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>0202</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="微軟正黑體"/>
-        <family val="2"/>
-        <charset val="136"/>
-      </rPr>
-      <t>】請確認中央上層筋下限，是否符合規範</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> 15.4.2.1 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="微軟正黑體"/>
-        <family val="2"/>
-        <charset val="136"/>
-      </rPr>
-      <t>規定</t>
-    </r>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>0203</t>
   </si>
   <si>
@@ -4678,6 +4627,57 @@
         <family val="2"/>
       </rPr>
       <t xml:space="preserve"> 30cm</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>【</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>0202</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>】請確認中央上層筋下限，是否符合規範</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 3.6 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>規定</t>
     </r>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -5822,8 +5822,8 @@
   <sheetPr codeName="工作表2"/>
   <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="G2:I2"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -5982,13 +5982,13 @@
         <v>52</v>
       </c>
       <c r="L5" s="39" t="s">
-        <v>57</v>
+        <v>188</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A6" s="21"/>
       <c r="B6" s="31" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C6" s="23">
         <v>1</v>
@@ -6002,7 +6002,7 @@
         <v>48</v>
       </c>
       <c r="H6" s="27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I6" s="27" t="s">
         <v>50</v>
@@ -6014,13 +6014,13 @@
         <v>52</v>
       </c>
       <c r="L6" s="37" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A7" s="21"/>
       <c r="B7" s="31" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C7" s="23">
         <v>1</v>
@@ -6037,7 +6037,7 @@
         <v>49</v>
       </c>
       <c r="I7" s="27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J7" s="38" t="s">
         <v>51</v>
@@ -6046,13 +6046,13 @@
         <v>52</v>
       </c>
       <c r="L7" s="37" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A8" s="21"/>
       <c r="B8" s="31" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C8" s="23">
         <v>1</v>
@@ -6069,7 +6069,7 @@
         <v>56</v>
       </c>
       <c r="I8" s="27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J8" s="38" t="s">
         <v>51</v>
@@ -6078,13 +6078,13 @@
         <v>52</v>
       </c>
       <c r="L8" s="37" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A9" s="21"/>
       <c r="B9" s="31" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C9" s="23">
         <v>1</v>
@@ -6098,10 +6098,10 @@
         <v>48</v>
       </c>
       <c r="H9" s="27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I9" s="27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J9" s="38" t="s">
         <v>51</v>
@@ -6110,13 +6110,13 @@
         <v>52</v>
       </c>
       <c r="L9" s="37" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A10" s="21"/>
       <c r="B10" s="31" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C10" s="23">
         <v>1</v>
@@ -6128,23 +6128,23 @@
       </c>
       <c r="G10" s="27"/>
       <c r="H10" s="27" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I10" s="27"/>
       <c r="J10" s="38" t="s">
+        <v>69</v>
+      </c>
+      <c r="K10" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="K10" s="29" t="s">
+      <c r="L10" s="37" t="s">
         <v>71</v>
-      </c>
-      <c r="L10" s="37" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A11" s="21"/>
       <c r="B11" s="31" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C11" s="23">
         <v>1</v>
@@ -6155,22 +6155,22 @@
         <v>16</v>
       </c>
       <c r="G11" s="27" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H11" s="27"/>
       <c r="I11" s="27"/>
       <c r="J11" s="38"/>
       <c r="K11" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="L11" s="39" t="s">
         <v>75</v>
-      </c>
-      <c r="L11" s="39" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A12" s="21"/>
       <c r="B12" s="31" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C12" s="23">
         <v>1</v>
@@ -6189,16 +6189,16 @@
         <v>35</v>
       </c>
       <c r="K12" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="L12" s="37" t="s">
         <v>78</v>
-      </c>
-      <c r="L12" s="37" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A13" s="21"/>
       <c r="B13" s="31" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C13" s="23">
         <v>1</v>
@@ -6210,23 +6210,23 @@
       </c>
       <c r="G13" s="27"/>
       <c r="H13" s="27" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I13" s="27"/>
       <c r="J13" s="38" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K13" s="29" t="s">
+        <v>81</v>
+      </c>
+      <c r="L13" s="37" t="s">
         <v>82</v>
-      </c>
-      <c r="L13" s="37" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A14" s="21"/>
       <c r="B14" s="31" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C14" s="23">
         <v>1</v>
@@ -6238,23 +6238,23 @@
       </c>
       <c r="G14" s="27"/>
       <c r="H14" s="27" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I14" s="27"/>
       <c r="J14" s="38" t="s">
         <v>51</v>
       </c>
       <c r="K14" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="L14" s="37" t="s">
         <v>85</v>
-      </c>
-      <c r="L14" s="37" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A15" s="21"/>
       <c r="B15" s="31" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C15" s="23">
         <v>1</v>
@@ -6274,19 +6274,19 @@
         <v>50</v>
       </c>
       <c r="J15" s="38" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K15" s="29" t="s">
+        <v>87</v>
+      </c>
+      <c r="L15" s="37" t="s">
         <v>88</v>
-      </c>
-      <c r="L15" s="37" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A16" s="21"/>
       <c r="B16" s="31" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C16" s="23">
         <v>1</v>
@@ -6306,19 +6306,19 @@
         <v>50</v>
       </c>
       <c r="J16" s="38" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K16" s="29" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="L16" s="37" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A17" s="21"/>
       <c r="B17" s="31" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C17" s="23">
         <v>1</v>
@@ -6332,25 +6332,25 @@
         <v>48</v>
       </c>
       <c r="H17" s="27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I17" s="27" t="s">
         <v>50</v>
       </c>
       <c r="J17" s="38" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K17" s="29" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="L17" s="37" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A18" s="21"/>
       <c r="B18" s="31" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C18" s="23">
         <v>1</v>
@@ -6367,22 +6367,22 @@
         <v>49</v>
       </c>
       <c r="I18" s="27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J18" s="38" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K18" s="29" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="L18" s="37" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A19" s="21"/>
       <c r="B19" s="31" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C19" s="23">
         <v>1</v>
@@ -6399,22 +6399,22 @@
         <v>56</v>
       </c>
       <c r="I19" s="27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J19" s="38" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K19" s="29" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="L19" s="37" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A20" s="21"/>
       <c r="B20" s="31" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C20" s="23">
         <v>1</v>
@@ -6428,25 +6428,25 @@
         <v>48</v>
       </c>
       <c r="H20" s="27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I20" s="27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J20" s="38" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K20" s="29" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="L20" s="37" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A21" s="21"/>
       <c r="B21" s="31" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C21" s="23">
         <v>1</v>
@@ -6462,19 +6462,19 @@
       <c r="H21" s="27"/>
       <c r="I21" s="27"/>
       <c r="J21" s="38" t="s">
+        <v>100</v>
+      </c>
+      <c r="K21" s="35" t="s">
+        <v>115</v>
+      </c>
+      <c r="L21" s="37" t="s">
         <v>101</v>
-      </c>
-      <c r="K21" s="35" t="s">
-        <v>116</v>
-      </c>
-      <c r="L21" s="37" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A22" s="21"/>
       <c r="B22" s="31" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C22" s="23">
         <v>1</v>
@@ -6488,23 +6488,23 @@
       </c>
       <c r="G22" s="27"/>
       <c r="H22" s="34" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I22" s="34"/>
       <c r="J22" s="38" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="K22" s="40" t="s">
+        <v>104</v>
+      </c>
+      <c r="L22" s="37" t="s">
         <v>105</v>
-      </c>
-      <c r="L22" s="37" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A23" s="21"/>
       <c r="B23" s="31" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C23" s="23">
         <v>1</v>
@@ -6518,23 +6518,23 @@
       </c>
       <c r="G23" s="34"/>
       <c r="H23" s="34" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I23" s="34"/>
       <c r="J23" s="38" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K23" s="40" t="s">
+        <v>107</v>
+      </c>
+      <c r="L23" s="37" t="s">
         <v>108</v>
-      </c>
-      <c r="L23" s="37" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="24" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A24" s="21"/>
       <c r="B24" s="31" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C24" s="23"/>
       <c r="D24" s="24">
@@ -6554,19 +6554,19 @@
         <v>50</v>
       </c>
       <c r="J24" s="38" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K24" s="29" t="s">
+        <v>110</v>
+      </c>
+      <c r="L24" s="37" t="s">
         <v>111</v>
-      </c>
-      <c r="L24" s="37" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="25" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A25" s="21"/>
       <c r="B25" s="42" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C25" s="23">
         <v>1</v>
@@ -6577,20 +6577,20 @@
         <v>16</v>
       </c>
       <c r="G25" s="27" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H25" s="34"/>
       <c r="I25" s="34" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J25" s="38" t="s">
         <v>51</v>
       </c>
       <c r="K25" s="40" t="s">
+        <v>113</v>
+      </c>
+      <c r="L25" s="41" t="s">
         <v>114</v>
-      </c>
-      <c r="L25" s="41" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="26" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
@@ -6675,10 +6675,10 @@
     </row>
     <row r="2" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="47" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C2" s="13" t="s">
         <v>12</v>
@@ -6719,10 +6719,10 @@
     </row>
     <row r="4" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
+        <v>118</v>
+      </c>
+      <c r="B4" s="31" t="s">
         <v>119</v>
-      </c>
-      <c r="B4" s="31" t="s">
-        <v>120</v>
       </c>
       <c r="C4" s="23">
         <v>1</v>
@@ -6748,15 +6748,15 @@
         <v>52</v>
       </c>
       <c r="L4" s="39" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A5" s="21" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B5" s="31" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C5" s="23">
         <v>1</v>
@@ -6782,15 +6782,15 @@
         <v>52</v>
       </c>
       <c r="L5" s="37" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A6" s="21" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B6" s="31" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C6" s="23">
         <v>1</v>
@@ -6804,7 +6804,7 @@
         <v>48</v>
       </c>
       <c r="H6" s="27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I6" s="27" t="s">
         <v>50</v>
@@ -6816,15 +6816,15 @@
         <v>52</v>
       </c>
       <c r="L6" s="37" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A7" s="21" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B7" s="31" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C7" s="23">
         <v>1</v>
@@ -6841,7 +6841,7 @@
         <v>49</v>
       </c>
       <c r="I7" s="27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J7" s="38" t="s">
         <v>51</v>
@@ -6850,13 +6850,13 @@
         <v>52</v>
       </c>
       <c r="L7" s="37" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A8" s="21"/>
       <c r="B8" s="31" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C8" s="23">
         <v>1</v>
@@ -6873,7 +6873,7 @@
         <v>56</v>
       </c>
       <c r="I8" s="27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J8" s="38" t="s">
         <v>51</v>
@@ -6882,15 +6882,15 @@
         <v>52</v>
       </c>
       <c r="L8" s="37" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A9" s="21" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B9" s="31" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C9" s="23">
         <v>1</v>
@@ -6904,10 +6904,10 @@
         <v>48</v>
       </c>
       <c r="H9" s="27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I9" s="27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J9" s="38" t="s">
         <v>51</v>
@@ -6916,13 +6916,13 @@
         <v>52</v>
       </c>
       <c r="L9" s="37" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A10" s="21"/>
       <c r="B10" s="31" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C10" s="23">
         <v>1</v>
@@ -6934,23 +6934,23 @@
       </c>
       <c r="G10" s="27"/>
       <c r="H10" s="27" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I10" s="27"/>
       <c r="J10" s="38" t="s">
+        <v>69</v>
+      </c>
+      <c r="K10" s="46" t="s">
         <v>70</v>
       </c>
-      <c r="K10" s="46" t="s">
-        <v>71</v>
-      </c>
       <c r="L10" s="37" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A11" s="21"/>
       <c r="B11" s="31" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C11" s="23">
         <v>1</v>
@@ -6962,23 +6962,23 @@
       </c>
       <c r="G11" s="27"/>
       <c r="H11" s="27" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I11" s="27"/>
       <c r="J11" s="38" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K11" s="29" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L11" s="37" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A12" s="21"/>
       <c r="B12" s="31" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C12" s="23">
         <v>1</v>
@@ -6990,23 +6990,23 @@
       </c>
       <c r="G12" s="27"/>
       <c r="H12" s="27" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I12" s="27"/>
       <c r="J12" s="38" t="s">
         <v>51</v>
       </c>
       <c r="K12" s="29" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L12" s="37" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A13" s="21"/>
       <c r="B13" s="31" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C13" s="23">
         <v>1</v>
@@ -7024,19 +7024,19 @@
         <v>50</v>
       </c>
       <c r="J13" s="38" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K13" s="29" t="s">
+        <v>138</v>
+      </c>
+      <c r="L13" s="37" t="s">
         <v>139</v>
-      </c>
-      <c r="L13" s="37" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A14" s="21"/>
       <c r="B14" s="31" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C14" s="23">
         <v>1</v>
@@ -7051,22 +7051,22 @@
       </c>
       <c r="H14" s="27"/>
       <c r="I14" s="27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J14" s="38" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K14" s="29" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="L14" s="37" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A15" s="21"/>
       <c r="B15" s="31" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C15" s="23">
         <v>1</v>
@@ -7078,17 +7078,17 @@
       </c>
       <c r="G15" s="45"/>
       <c r="H15" s="27" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I15" s="45"/>
       <c r="J15" s="38" t="s">
         <v>51</v>
       </c>
       <c r="K15" s="29" t="s">
+        <v>144</v>
+      </c>
+      <c r="L15" s="37" t="s">
         <v>145</v>
-      </c>
-      <c r="L15" s="37" t="s">
-        <v>146</v>
       </c>
     </row>
   </sheetData>
@@ -7102,7 +7102,7 @@
   <sheetPr codeName="工作表5"/>
   <dimension ref="A1:L17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
@@ -7159,10 +7159,10 @@
     </row>
     <row r="2" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="B2" s="12" t="s">
         <v>148</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>149</v>
       </c>
       <c r="C2" s="13" t="s">
         <v>12</v>
@@ -7204,7 +7204,7 @@
     <row r="4" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A4" s="21"/>
       <c r="B4" s="31" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C4" s="23">
         <v>1</v>
@@ -7215,7 +7215,7 @@
         <v>16</v>
       </c>
       <c r="G4" s="27" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H4" s="34"/>
       <c r="I4" s="34" t="s">
@@ -7225,16 +7225,16 @@
         <v>51</v>
       </c>
       <c r="K4" s="29" t="s">
+        <v>150</v>
+      </c>
+      <c r="L4" s="37" t="s">
         <v>151</v>
-      </c>
-      <c r="L4" s="37" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A5" s="21"/>
       <c r="B5" s="31" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C5" s="23">
         <v>1</v>
@@ -7245,26 +7245,26 @@
         <v>16</v>
       </c>
       <c r="G5" s="27" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H5" s="34"/>
       <c r="I5" s="34" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J5" s="38" t="s">
         <v>51</v>
       </c>
       <c r="K5" s="40" t="s">
+        <v>113</v>
+      </c>
+      <c r="L5" s="41" t="s">
         <v>114</v>
-      </c>
-      <c r="L5" s="41" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A6" s="21"/>
       <c r="B6" s="31" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C6" s="23"/>
       <c r="D6" s="24">
@@ -7275,26 +7275,26 @@
         <v>16</v>
       </c>
       <c r="G6" s="27" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H6" s="34"/>
       <c r="I6" s="34" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J6" s="38" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K6" s="40" t="s">
+        <v>154</v>
+      </c>
+      <c r="L6" s="41" t="s">
         <v>155</v>
-      </c>
-      <c r="L6" s="41" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A7" s="21"/>
       <c r="B7" s="31" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C7" s="23">
         <v>1</v>
@@ -7312,19 +7312,19 @@
         <v>50</v>
       </c>
       <c r="J7" s="38" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="K7" s="40" t="s">
+        <v>157</v>
+      </c>
+      <c r="L7" s="41" t="s">
         <v>158</v>
-      </c>
-      <c r="L7" s="41" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A8" s="21"/>
       <c r="B8" s="31" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C8" s="23">
         <v>1</v>
@@ -7339,22 +7339,22 @@
       </c>
       <c r="H8" s="27"/>
       <c r="I8" s="27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J8" s="38" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="K8" s="40" t="s">
+        <v>160</v>
+      </c>
+      <c r="L8" s="41" t="s">
         <v>161</v>
-      </c>
-      <c r="L8" s="41" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A9" s="21"/>
       <c r="B9" s="31" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C9" s="23">
         <v>1</v>
@@ -7366,23 +7366,23 @@
       </c>
       <c r="G9" s="27"/>
       <c r="H9" s="27" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="I9" s="34"/>
       <c r="J9" s="38" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K9" s="40" t="s">
+        <v>164</v>
+      </c>
+      <c r="L9" s="41" t="s">
         <v>165</v>
-      </c>
-      <c r="L9" s="41" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A10" s="21"/>
       <c r="B10" s="31" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C10" s="23">
         <v>1</v>
@@ -7394,23 +7394,23 @@
       </c>
       <c r="G10" s="27"/>
       <c r="H10" s="27" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="I10" s="34"/>
       <c r="J10" s="38" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="K10" s="40" t="s">
+        <v>167</v>
+      </c>
+      <c r="L10" s="41" t="s">
         <v>168</v>
-      </c>
-      <c r="L10" s="41" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A11" s="21"/>
       <c r="B11" s="31" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C11" s="23">
         <v>1</v>
@@ -7428,19 +7428,19 @@
         <v>50</v>
       </c>
       <c r="J11" s="38" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K11" s="40" t="s">
+        <v>170</v>
+      </c>
+      <c r="L11" s="41" t="s">
         <v>171</v>
-      </c>
-      <c r="L11" s="41" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A12" s="21"/>
       <c r="B12" s="31" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C12" s="23">
         <v>1</v>
@@ -7455,22 +7455,22 @@
       </c>
       <c r="H12" s="27"/>
       <c r="I12" s="27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J12" s="38" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K12" s="40" t="s">
+        <v>173</v>
+      </c>
+      <c r="L12" s="41" t="s">
         <v>174</v>
-      </c>
-      <c r="L12" s="41" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A13" s="21"/>
       <c r="B13" s="31" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C13" s="23"/>
       <c r="D13" s="24">
@@ -7487,22 +7487,22 @@
         <v>56</v>
       </c>
       <c r="I13" s="27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J13" s="38" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K13" s="40" t="s">
+        <v>176</v>
+      </c>
+      <c r="L13" s="41" t="s">
         <v>177</v>
-      </c>
-      <c r="L13" s="41" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A14" s="21"/>
       <c r="B14" s="31" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C14" s="23"/>
       <c r="D14" s="24">
@@ -7522,19 +7522,19 @@
         <v>50</v>
       </c>
       <c r="J14" s="38" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K14" s="40" t="s">
+        <v>179</v>
+      </c>
+      <c r="L14" s="41" t="s">
         <v>180</v>
-      </c>
-      <c r="L14" s="41" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A15" s="21"/>
       <c r="B15" s="31" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C15" s="23"/>
       <c r="D15" s="24">
@@ -7548,25 +7548,25 @@
         <v>48</v>
       </c>
       <c r="H15" s="27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I15" s="27" t="s">
         <v>50</v>
       </c>
       <c r="J15" s="38" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K15" s="40" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="L15" s="41" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A16" s="21"/>
       <c r="B16" s="31" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C16" s="23">
         <v>1</v>
@@ -7580,23 +7580,23 @@
       </c>
       <c r="G16" s="27"/>
       <c r="H16" s="34" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I16" s="34"/>
       <c r="J16" s="38" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="K16" s="40" t="s">
+        <v>184</v>
+      </c>
+      <c r="L16" s="41" t="s">
         <v>185</v>
-      </c>
-      <c r="L16" s="41" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A17" s="21"/>
       <c r="B17" s="31" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C17" s="23">
         <v>1</v>
@@ -7610,17 +7610,17 @@
       </c>
       <c r="G17" s="34"/>
       <c r="H17" s="34" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I17" s="34"/>
       <c r="J17" s="38" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K17" s="40" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="L17" s="41" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix tool2 html alse plan count
</commit_message>
<xml_diff>
--- a/file/柱SCAN.xlsx
+++ b/file/柱SCAN.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\BeamQC\file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DA6536F-F9F5-45F1-BB65-BD84F4645151}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D25E13A-2381-408C-8342-567CAC3A8868}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{8C2A7BE7-2142-4FCC-89B4-3B139FDB86C0}"/>
   </bookViews>
@@ -3234,9 +3234,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>0307</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <sz val="12"/>
@@ -5124,6 +5121,10 @@
   </si>
   <si>
     <t>0205</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0207</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -6110,7 +6111,7 @@
       </c>
       <c r="I6" s="27"/>
       <c r="J6" s="60" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="K6" s="35" t="s">
         <v>28</v>
@@ -6234,7 +6235,7 @@
     <row r="11" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A11" s="21"/>
       <c r="B11" s="31" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C11" s="23"/>
       <c r="D11" s="24"/>
@@ -6246,23 +6247,23 @@
       </c>
       <c r="G11" s="27"/>
       <c r="H11" s="58" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I11" s="27"/>
       <c r="J11" s="59" t="s">
+        <v>193</v>
+      </c>
+      <c r="K11" s="55" t="s">
         <v>194</v>
       </c>
-      <c r="K11" s="55" t="s">
+      <c r="L11" s="36" t="s">
         <v>195</v>
-      </c>
-      <c r="L11" s="36" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A12" s="21"/>
       <c r="B12" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C12" s="23">
         <v>1</v>
@@ -6276,23 +6277,23 @@
       </c>
       <c r="G12" s="27"/>
       <c r="H12" s="58" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="I12" s="27"/>
       <c r="J12" s="28" t="s">
         <v>35</v>
       </c>
       <c r="K12" s="55" t="s">
+        <v>201</v>
+      </c>
+      <c r="L12" s="36" t="s">
         <v>202</v>
-      </c>
-      <c r="L12" s="36" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A13" s="21"/>
       <c r="B13" s="31" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C13" s="23">
         <v>1</v>
@@ -6306,17 +6307,17 @@
       </c>
       <c r="G13" s="27"/>
       <c r="H13" s="58" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="I13" s="27"/>
       <c r="J13" s="28" t="s">
         <v>35</v>
       </c>
       <c r="K13" s="55" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="L13" s="36" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
@@ -6518,7 +6519,7 @@
         <v>52</v>
       </c>
       <c r="L5" s="39" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
@@ -7132,7 +7133,7 @@
     <row r="26" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A26" s="21"/>
       <c r="B26" s="42" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C26" s="23"/>
       <c r="D26" s="24"/>
@@ -7151,10 +7152,10 @@
         <v>51</v>
       </c>
       <c r="K26" s="40" t="s">
+        <v>188</v>
+      </c>
+      <c r="L26" s="39" t="s">
         <v>189</v>
-      </c>
-      <c r="L26" s="39" t="s">
-        <v>190</v>
       </c>
     </row>
   </sheetData>
@@ -7169,7 +7170,7 @@
   <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -7225,7 +7226,7 @@
     </row>
     <row r="2" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="47" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>117</v>
@@ -7406,7 +7407,7 @@
     <row r="8" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A8" s="21"/>
       <c r="B8" s="42" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C8" s="23">
         <v>1</v>
@@ -7471,8 +7472,8 @@
     </row>
     <row r="10" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A10" s="21"/>
-      <c r="B10" s="31" t="s">
-        <v>130</v>
+      <c r="B10" s="42" t="s">
+        <v>206</v>
       </c>
       <c r="C10" s="23">
         <v>1</v>
@@ -7494,13 +7495,13 @@
         <v>70</v>
       </c>
       <c r="L10" s="37" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A11" s="21"/>
       <c r="B11" s="31" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C11" s="23">
         <v>1</v>
@@ -7522,13 +7523,13 @@
         <v>81</v>
       </c>
       <c r="L11" s="37" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A12" s="21"/>
       <c r="B12" s="31" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C12" s="23">
         <v>1</v>
@@ -7550,13 +7551,13 @@
         <v>84</v>
       </c>
       <c r="L12" s="37" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A13" s="21"/>
       <c r="B13" s="31" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C13" s="23">
         <v>1</v>
@@ -7577,16 +7578,16 @@
         <v>69</v>
       </c>
       <c r="K13" s="29" t="s">
+        <v>136</v>
+      </c>
+      <c r="L13" s="37" t="s">
         <v>137</v>
-      </c>
-      <c r="L13" s="37" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A14" s="21"/>
       <c r="B14" s="31" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C14" s="23">
         <v>1</v>
@@ -7607,16 +7608,16 @@
         <v>69</v>
       </c>
       <c r="K14" s="29" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L14" s="37" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A15" s="21"/>
       <c r="B15" s="31" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C15" s="23">
         <v>1</v>
@@ -7628,23 +7629,23 @@
       </c>
       <c r="G15" s="45"/>
       <c r="H15" s="27" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I15" s="45"/>
       <c r="J15" s="38" t="s">
         <v>51</v>
       </c>
       <c r="K15" s="29" t="s">
+        <v>142</v>
+      </c>
+      <c r="L15" s="37" t="s">
         <v>143</v>
-      </c>
-      <c r="L15" s="37" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A16" s="21"/>
       <c r="B16" s="31" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C16" s="23">
         <v>1</v>
@@ -7663,10 +7664,10 @@
         <v>51</v>
       </c>
       <c r="K16" s="57" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="L16" s="39" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
   </sheetData>
@@ -7737,10 +7738,10 @@
     </row>
     <row r="2" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="B2" s="12" t="s">
         <v>146</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>147</v>
       </c>
       <c r="C2" s="13" t="s">
         <v>12</v>
@@ -7782,7 +7783,7 @@
     <row r="4" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A4" s="21"/>
       <c r="B4" s="31" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C4" s="23">
         <v>1</v>
@@ -7803,16 +7804,16 @@
         <v>51</v>
       </c>
       <c r="K4" s="29" t="s">
+        <v>148</v>
+      </c>
+      <c r="L4" s="37" t="s">
         <v>149</v>
-      </c>
-      <c r="L4" s="37" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A5" s="21"/>
       <c r="B5" s="31" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C5" s="23">
         <v>1</v>
@@ -7842,7 +7843,7 @@
     <row r="6" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A6" s="21"/>
       <c r="B6" s="31" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C6" s="23"/>
       <c r="D6" s="24">
@@ -7863,16 +7864,16 @@
         <v>69</v>
       </c>
       <c r="K6" s="40" t="s">
+        <v>152</v>
+      </c>
+      <c r="L6" s="41" t="s">
         <v>153</v>
-      </c>
-      <c r="L6" s="41" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A7" s="21"/>
       <c r="B7" s="31" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C7" s="23">
         <v>1</v>
@@ -7893,16 +7894,16 @@
         <v>100</v>
       </c>
       <c r="K7" s="40" t="s">
+        <v>155</v>
+      </c>
+      <c r="L7" s="41" t="s">
         <v>156</v>
-      </c>
-      <c r="L7" s="41" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A8" s="21"/>
       <c r="B8" s="31" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C8" s="23">
         <v>1</v>
@@ -7923,16 +7924,16 @@
         <v>100</v>
       </c>
       <c r="K8" s="40" t="s">
+        <v>158</v>
+      </c>
+      <c r="L8" s="41" t="s">
         <v>159</v>
-      </c>
-      <c r="L8" s="41" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A9" s="21"/>
       <c r="B9" s="31" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C9" s="23">
         <v>1</v>
@@ -7944,23 +7945,23 @@
       </c>
       <c r="G9" s="27"/>
       <c r="H9" s="27" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="I9" s="34"/>
       <c r="J9" s="38" t="s">
         <v>69</v>
       </c>
       <c r="K9" s="40" t="s">
+        <v>162</v>
+      </c>
+      <c r="L9" s="41" t="s">
         <v>163</v>
-      </c>
-      <c r="L9" s="41" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A10" s="21"/>
       <c r="B10" s="31" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C10" s="23">
         <v>1</v>
@@ -7972,23 +7973,23 @@
       </c>
       <c r="G10" s="27"/>
       <c r="H10" s="27" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="I10" s="34"/>
       <c r="J10" s="38" t="s">
         <v>100</v>
       </c>
       <c r="K10" s="40" t="s">
+        <v>165</v>
+      </c>
+      <c r="L10" s="41" t="s">
         <v>166</v>
-      </c>
-      <c r="L10" s="41" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A11" s="21"/>
       <c r="B11" s="31" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C11" s="23">
         <v>1</v>
@@ -8009,16 +8010,16 @@
         <v>69</v>
       </c>
       <c r="K11" s="40" t="s">
+        <v>168</v>
+      </c>
+      <c r="L11" s="41" t="s">
         <v>169</v>
-      </c>
-      <c r="L11" s="41" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A12" s="21"/>
       <c r="B12" s="31" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C12" s="23">
         <v>1</v>
@@ -8039,16 +8040,16 @@
         <v>69</v>
       </c>
       <c r="K12" s="40" t="s">
+        <v>171</v>
+      </c>
+      <c r="L12" s="41" t="s">
         <v>172</v>
-      </c>
-      <c r="L12" s="41" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A13" s="21"/>
       <c r="B13" s="31" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C13" s="23"/>
       <c r="D13" s="24">
@@ -8071,16 +8072,16 @@
         <v>69</v>
       </c>
       <c r="K13" s="40" t="s">
+        <v>174</v>
+      </c>
+      <c r="L13" s="41" t="s">
         <v>175</v>
-      </c>
-      <c r="L13" s="41" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A14" s="21"/>
       <c r="B14" s="31" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C14" s="23"/>
       <c r="D14" s="24">
@@ -8103,16 +8104,16 @@
         <v>69</v>
       </c>
       <c r="K14" s="40" t="s">
+        <v>177</v>
+      </c>
+      <c r="L14" s="41" t="s">
         <v>178</v>
-      </c>
-      <c r="L14" s="41" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A15" s="21"/>
       <c r="B15" s="31" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C15" s="23"/>
       <c r="D15" s="24">
@@ -8135,16 +8136,16 @@
         <v>69</v>
       </c>
       <c r="K15" s="40" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="L15" s="41" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A16" s="21"/>
       <c r="B16" s="31" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C16" s="23">
         <v>1</v>
@@ -8165,16 +8166,16 @@
         <v>100</v>
       </c>
       <c r="K16" s="40" t="s">
+        <v>182</v>
+      </c>
+      <c r="L16" s="41" t="s">
         <v>183</v>
-      </c>
-      <c r="L16" s="41" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A17" s="21"/>
       <c r="B17" s="31" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C17" s="23">
         <v>1</v>
@@ -8198,7 +8199,7 @@
         <v>107</v>
       </c>
       <c r="L17" s="41" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add column beam joint
</commit_message>
<xml_diff>
--- a/file/柱SCAN.xlsx
+++ b/file/柱SCAN.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\BeamQC\file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D25E13A-2381-408C-8342-567CAC3A8868}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{663586D9-BD5C-4D10-BB3A-0A12380DE2A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{8C2A7BE7-2142-4FCC-89B4-3B139FDB86C0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8C2A7BE7-2142-4FCC-89B4-3B139FDB86C0}"/>
   </bookViews>
   <sheets>
     <sheet name="柱" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="216">
   <si>
     <t>Type</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -5125,6 +5125,133 @@
   </si>
   <si>
     <t>0207</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>箍筋</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>上限</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>中央箍筋應考慮混凝土貢獻</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0224</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>【</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>0224</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>】</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Microsoft JhengHei"/>
+        <family val="3"/>
+      </rPr>
+      <t>中央箍筋超過</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="3"/>
+      </rPr>
+      <t>1.5</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Microsoft JhengHei"/>
+        <family val="3"/>
+      </rPr>
+      <t>倍需求</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>接頭剪力</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0411</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>接頭剪力符合規範</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>【</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>0411</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>】</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Microsoft JhengHei"/>
+        <family val="2"/>
+      </rPr>
+      <t>接頭未符合規範接頭剪力需求</t>
+    </r>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -5132,7 +5259,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="18">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -5226,6 +5353,29 @@
       <name val="新細明體"/>
       <family val="3"/>
       <charset val="136"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Microsoft JhengHei"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Microsoft JhengHei"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Microsoft JhengHei"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="11">
@@ -5431,7 +5581,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -5615,6 +5765,15 @@
     <xf numFmtId="0" fontId="5" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
@@ -5633,9 +5792,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 佈景主題">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 主題">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -5673,7 +5832,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -5779,7 +5938,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -5921,7 +6080,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -5932,11 +6091,11 @@
   <sheetPr codeName="工作表1"/>
   <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="1" width="8.875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.5" bestFit="1" customWidth="1"/>
@@ -5950,7 +6109,7 @@
     <col min="12" max="12" width="57.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="18.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5988,7 +6147,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="19.5" thickBot="1">
       <c r="A2" s="11" t="s">
         <v>10</v>
       </c>
@@ -6018,7 +6177,7 @@
       <c r="K2" s="19"/>
       <c r="L2" s="20"/>
     </row>
-    <row r="3" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="18.75">
       <c r="A3" s="21"/>
       <c r="B3" s="22"/>
       <c r="C3" s="23"/>
@@ -6032,7 +6191,7 @@
       <c r="K3" s="29"/>
       <c r="L3" s="30"/>
     </row>
-    <row r="4" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="18.75">
       <c r="A4" s="21"/>
       <c r="B4" s="31" t="s">
         <v>15</v>
@@ -6062,7 +6221,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="18.75">
       <c r="A5" s="21"/>
       <c r="B5" s="31" t="s">
         <v>21</v>
@@ -6092,7 +6251,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="18.75">
       <c r="A6" s="21"/>
       <c r="B6" s="31" t="s">
         <v>25</v>
@@ -6120,7 +6279,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="18.75">
       <c r="A7" s="21"/>
       <c r="B7" s="31" t="s">
         <v>30</v>
@@ -6148,7 +6307,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="18.75">
       <c r="A8" s="21"/>
       <c r="B8" s="31" t="s">
         <v>33</v>
@@ -6176,7 +6335,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="18.75">
       <c r="A9" s="21"/>
       <c r="B9" s="31" t="s">
         <v>38</v>
@@ -6204,7 +6363,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" ht="18.75">
       <c r="A10" s="21"/>
       <c r="B10" s="31" t="s">
         <v>42</v>
@@ -6232,7 +6391,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" ht="18.75">
       <c r="A11" s="21"/>
       <c r="B11" s="31" t="s">
         <v>199</v>
@@ -6260,7 +6419,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" ht="18.75">
       <c r="A12" s="21"/>
       <c r="B12" s="31" t="s">
         <v>200</v>
@@ -6290,7 +6449,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" ht="18.75">
       <c r="A13" s="21"/>
       <c r="B13" s="31" t="s">
         <v>203</v>
@@ -6320,21 +6479,37 @@
         <v>204</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" ht="18.75">
       <c r="A14" s="21"/>
-      <c r="B14" s="22"/>
-      <c r="C14" s="23"/>
+      <c r="B14" s="31" t="s">
+        <v>213</v>
+      </c>
+      <c r="C14" s="23">
+        <v>1</v>
+      </c>
       <c r="D14" s="24"/>
-      <c r="E14" s="25"/>
-      <c r="F14" s="26"/>
+      <c r="E14" s="25">
+        <v>1</v>
+      </c>
+      <c r="F14" s="32" t="s">
+        <v>16</v>
+      </c>
       <c r="G14" s="27"/>
-      <c r="H14" s="27"/>
+      <c r="H14" s="58" t="s">
+        <v>212</v>
+      </c>
       <c r="I14" s="27"/>
-      <c r="J14" s="28"/>
-      <c r="K14" s="29"/>
-      <c r="L14" s="30"/>
+      <c r="J14" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="K14" s="55" t="s">
+        <v>214</v>
+      </c>
+      <c r="L14" s="36" t="s">
+        <v>215</v>
+      </c>
     </row>
-    <row r="15" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" ht="18.75">
       <c r="A15" s="21"/>
       <c r="B15" s="22"/>
       <c r="C15" s="23"/>
@@ -6357,13 +6532,13 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8018E948-6A60-4E64-8396-6BA3DA348946}">
   <sheetPr codeName="工作表2"/>
-  <dimension ref="A1:L26"/>
+  <dimension ref="A1:L27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L31" sqref="L31"/>
+      <selection activeCell="L29" sqref="L29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="1" width="6.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.5" bestFit="1" customWidth="1"/>
@@ -6376,7 +6551,7 @@
     <col min="12" max="12" width="98.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="18.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6414,7 +6589,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="19.5" thickBot="1">
       <c r="A2" s="11" t="s">
         <v>45</v>
       </c>
@@ -6444,7 +6619,7 @@
       <c r="K2" s="19"/>
       <c r="L2" s="20"/>
     </row>
-    <row r="3" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="18.75">
       <c r="A3" s="21"/>
       <c r="B3" s="31"/>
       <c r="C3" s="23"/>
@@ -6458,7 +6633,7 @@
       <c r="K3" s="29"/>
       <c r="L3" s="37"/>
     </row>
-    <row r="4" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="18.75">
       <c r="A4" s="21"/>
       <c r="B4" s="31" t="s">
         <v>47</v>
@@ -6490,7 +6665,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="18.75">
       <c r="A5" s="21"/>
       <c r="B5" s="31" t="s">
         <v>54</v>
@@ -6522,7 +6697,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="18.75">
       <c r="A6" s="21"/>
       <c r="B6" s="31" t="s">
         <v>57</v>
@@ -6554,7 +6729,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="18.75">
       <c r="A7" s="21"/>
       <c r="B7" s="31" t="s">
         <v>60</v>
@@ -6586,7 +6761,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="18.75">
       <c r="A8" s="21"/>
       <c r="B8" s="31" t="s">
         <v>63</v>
@@ -6618,7 +6793,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="18.75">
       <c r="A9" s="21"/>
       <c r="B9" s="31" t="s">
         <v>65</v>
@@ -6650,7 +6825,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" ht="18.75">
       <c r="A10" s="21"/>
       <c r="B10" s="31" t="s">
         <v>67</v>
@@ -6678,7 +6853,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" ht="18.75">
       <c r="A11" s="21"/>
       <c r="B11" s="31" t="s">
         <v>72</v>
@@ -6704,7 +6879,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" ht="18.75">
       <c r="A12" s="21"/>
       <c r="B12" s="31" t="s">
         <v>76</v>
@@ -6732,7 +6907,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" ht="18.75">
       <c r="A13" s="21"/>
       <c r="B13" s="31" t="s">
         <v>79</v>
@@ -6760,7 +6935,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" ht="18.75">
       <c r="A14" s="21"/>
       <c r="B14" s="31" t="s">
         <v>83</v>
@@ -6788,7 +6963,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" ht="18.75">
       <c r="A15" s="21"/>
       <c r="B15" s="31" t="s">
         <v>86</v>
@@ -6820,7 +6995,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" ht="18.75">
       <c r="A16" s="21"/>
       <c r="B16" s="31" t="s">
         <v>89</v>
@@ -6852,7 +7027,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" ht="18.75">
       <c r="A17" s="21"/>
       <c r="B17" s="31" t="s">
         <v>91</v>
@@ -6884,7 +7059,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" ht="18.75">
       <c r="A18" s="21"/>
       <c r="B18" s="31" t="s">
         <v>93</v>
@@ -6916,7 +7091,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" ht="18.75">
       <c r="A19" s="21"/>
       <c r="B19" s="31" t="s">
         <v>95</v>
@@ -6948,7 +7123,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" ht="18.75">
       <c r="A20" s="21"/>
       <c r="B20" s="31" t="s">
         <v>97</v>
@@ -6980,7 +7155,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" ht="18.75">
       <c r="A21" s="21"/>
       <c r="B21" s="31" t="s">
         <v>99</v>
@@ -7008,7 +7183,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" ht="18.75">
       <c r="A22" s="21"/>
       <c r="B22" s="31" t="s">
         <v>102</v>
@@ -7038,7 +7213,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" ht="18.75">
       <c r="A23" s="21"/>
       <c r="B23" s="31" t="s">
         <v>106</v>
@@ -7068,7 +7243,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" ht="18.75">
       <c r="A24" s="21"/>
       <c r="B24" s="31" t="s">
         <v>109</v>
@@ -7100,7 +7275,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" ht="18.75">
       <c r="A25" s="21"/>
       <c r="B25" s="42" t="s">
         <v>116</v>
@@ -7130,7 +7305,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" ht="18.75">
       <c r="A26" s="21"/>
       <c r="B26" s="42" t="s">
         <v>187</v>
@@ -7156,6 +7331,36 @@
       </c>
       <c r="L26" s="39" t="s">
         <v>189</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="18.75">
+      <c r="A27" s="21"/>
+      <c r="B27" s="42" t="s">
+        <v>210</v>
+      </c>
+      <c r="C27" s="23"/>
+      <c r="D27" s="24">
+        <v>1</v>
+      </c>
+      <c r="E27" s="25"/>
+      <c r="F27" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="G27" s="61" t="s">
+        <v>207</v>
+      </c>
+      <c r="H27" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="I27" s="27"/>
+      <c r="J27" s="62" t="s">
+        <v>208</v>
+      </c>
+      <c r="K27" s="63" t="s">
+        <v>209</v>
+      </c>
+      <c r="L27" s="39" t="s">
+        <v>211</v>
       </c>
     </row>
   </sheetData>
@@ -7169,11 +7374,11 @@
   <sheetPr codeName="工作表4"/>
   <dimension ref="A1:L16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="1" width="6.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.5" bestFit="1" customWidth="1"/>
@@ -7186,7 +7391,7 @@
     <col min="12" max="12" width="61.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="18.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -7224,7 +7429,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="19.5" thickBot="1">
       <c r="A2" s="47" t="s">
         <v>144</v>
       </c>
@@ -7254,7 +7459,7 @@
       <c r="K2" s="19"/>
       <c r="L2" s="20"/>
     </row>
-    <row r="3" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="18.75">
       <c r="A3" s="21"/>
       <c r="B3" s="31"/>
       <c r="C3" s="23"/>
@@ -7268,7 +7473,7 @@
       <c r="K3" s="29"/>
       <c r="L3" s="37"/>
     </row>
-    <row r="4" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="18.75">
       <c r="A4" s="21" t="s">
         <v>118</v>
       </c>
@@ -7302,7 +7507,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="18.75">
       <c r="A5" s="21" t="s">
         <v>118</v>
       </c>
@@ -7336,7 +7541,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="18.75">
       <c r="A6" s="21" t="s">
         <v>118</v>
       </c>
@@ -7370,7 +7575,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="18.75">
       <c r="A7" s="21" t="s">
         <v>118</v>
       </c>
@@ -7404,7 +7609,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="18.75">
       <c r="A8" s="21"/>
       <c r="B8" s="42" t="s">
         <v>205</v>
@@ -7436,7 +7641,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="18.75">
       <c r="A9" s="21" t="s">
         <v>118</v>
       </c>
@@ -7470,7 +7675,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" ht="31.5">
       <c r="A10" s="21"/>
       <c r="B10" s="42" t="s">
         <v>206</v>
@@ -7498,7 +7703,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" ht="18.75">
       <c r="A11" s="21"/>
       <c r="B11" s="31" t="s">
         <v>131</v>
@@ -7526,7 +7731,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" ht="18.75">
       <c r="A12" s="21"/>
       <c r="B12" s="31" t="s">
         <v>133</v>
@@ -7554,7 +7759,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" ht="18.75">
       <c r="A13" s="21"/>
       <c r="B13" s="31" t="s">
         <v>135</v>
@@ -7584,7 +7789,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" ht="18.75">
       <c r="A14" s="21"/>
       <c r="B14" s="31" t="s">
         <v>138</v>
@@ -7614,7 +7819,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" ht="18.75">
       <c r="A15" s="21"/>
       <c r="B15" s="31" t="s">
         <v>140</v>
@@ -7642,7 +7847,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" ht="18.75">
       <c r="A16" s="21"/>
       <c r="B16" s="31" t="s">
         <v>190</v>
@@ -7685,7 +7890,7 @@
       <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="1" width="6.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.5" bestFit="1" customWidth="1"/>
@@ -7698,7 +7903,7 @@
     <col min="12" max="12" width="53.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="18.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -7736,7 +7941,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="19.5" thickBot="1">
       <c r="A2" s="11" t="s">
         <v>145</v>
       </c>
@@ -7766,7 +7971,7 @@
       <c r="K2" s="19"/>
       <c r="L2" s="20"/>
     </row>
-    <row r="3" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="18.75">
       <c r="A3" s="21"/>
       <c r="B3" s="48"/>
       <c r="C3" s="49"/>
@@ -7780,7 +7985,7 @@
       <c r="K3" s="52"/>
       <c r="L3" s="53"/>
     </row>
-    <row r="4" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="18.75">
       <c r="A4" s="21"/>
       <c r="B4" s="31" t="s">
         <v>147</v>
@@ -7810,7 +8015,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="18.75">
       <c r="A5" s="21"/>
       <c r="B5" s="31" t="s">
         <v>150</v>
@@ -7840,7 +8045,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="18.75">
       <c r="A6" s="21"/>
       <c r="B6" s="31" t="s">
         <v>151</v>
@@ -7870,7 +8075,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="18.75">
       <c r="A7" s="21"/>
       <c r="B7" s="31" t="s">
         <v>154</v>
@@ -7900,7 +8105,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="18.75">
       <c r="A8" s="21"/>
       <c r="B8" s="31" t="s">
         <v>157</v>
@@ -7930,7 +8135,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="18.75">
       <c r="A9" s="21"/>
       <c r="B9" s="31" t="s">
         <v>160</v>
@@ -7958,7 +8163,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" ht="18.75">
       <c r="A10" s="21"/>
       <c r="B10" s="31" t="s">
         <v>164</v>
@@ -7986,7 +8191,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" ht="18.75">
       <c r="A11" s="21"/>
       <c r="B11" s="31" t="s">
         <v>167</v>
@@ -8016,7 +8221,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" ht="18.75">
       <c r="A12" s="21"/>
       <c r="B12" s="31" t="s">
         <v>170</v>
@@ -8046,7 +8251,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" ht="18.75">
       <c r="A13" s="21"/>
       <c r="B13" s="31" t="s">
         <v>173</v>
@@ -8078,7 +8283,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" ht="18.75">
       <c r="A14" s="21"/>
       <c r="B14" s="31" t="s">
         <v>176</v>
@@ -8110,7 +8315,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" ht="18.75">
       <c r="A15" s="21"/>
       <c r="B15" s="31" t="s">
         <v>179</v>
@@ -8142,7 +8347,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" ht="18.75">
       <c r="A16" s="21"/>
       <c r="B16" s="31" t="s">
         <v>181</v>
@@ -8172,7 +8377,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" ht="18.75">
       <c r="A17" s="21"/>
       <c r="B17" s="31" t="s">
         <v>184</v>

</xml_diff>

<commit_message>
fix:line order error rc scan
</commit_message>
<xml_diff>
--- a/file/柱SCAN.xlsx
+++ b/file/柱SCAN.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\BeamQC\file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55BBAA17-B273-4125-BA99-CF4C1C746EC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9606CA26-E23D-47C8-82F4-F10896049AF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{8C2A7BE7-2142-4FCC-89B4-3B139FDB86C0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{8C2A7BE7-2142-4FCC-89B4-3B139FDB86C0}"/>
   </bookViews>
   <sheets>
     <sheet name="柱" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="217">
   <si>
     <t>Type</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -6523,8 +6523,8 @@
   <sheetPr codeName="工作表2"/>
   <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -6655,7 +6655,9 @@
       </c>
     </row>
     <row r="5" spans="1:12" ht="18.75">
-      <c r="A5" s="21"/>
+      <c r="A5" s="21" t="s">
+        <v>101</v>
+      </c>
       <c r="B5" s="31" t="s">
         <v>51</v>
       </c>
@@ -6871,7 +6873,9 @@
       </c>
     </row>
     <row r="12" spans="1:12" ht="18.75">
-      <c r="A12" s="21"/>
+      <c r="A12" s="21" t="s">
+        <v>101</v>
+      </c>
       <c r="B12" s="31" t="s">
         <v>68</v>
       </c>
@@ -7365,7 +7369,7 @@
   <sheetPr codeName="工作表4"/>
   <dimension ref="A1:L16"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>
@@ -7877,8 +7881,8 @@
   <sheetPr codeName="工作表5"/>
   <dimension ref="A1:L17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -8067,7 +8071,9 @@
       </c>
     </row>
     <row r="7" spans="1:12" ht="18.75">
-      <c r="A7" s="21"/>
+      <c r="A7" s="21" t="s">
+        <v>101</v>
+      </c>
       <c r="B7" s="31" t="s">
         <v>134</v>
       </c>
@@ -8097,7 +8103,9 @@
       </c>
     </row>
     <row r="8" spans="1:12" ht="18.75">
-      <c r="A8" s="21"/>
+      <c r="A8" s="21" t="s">
+        <v>101</v>
+      </c>
       <c r="B8" s="31" t="s">
         <v>137</v>
       </c>
@@ -8183,7 +8191,9 @@
       </c>
     </row>
     <row r="11" spans="1:12" ht="18.75">
-      <c r="A11" s="21"/>
+      <c r="A11" s="21" t="s">
+        <v>101</v>
+      </c>
       <c r="B11" s="31" t="s">
         <v>147</v>
       </c>
@@ -8213,7 +8223,9 @@
       </c>
     </row>
     <row r="12" spans="1:12" ht="18.75">
-      <c r="A12" s="21"/>
+      <c r="A12" s="21" t="s">
+        <v>101</v>
+      </c>
       <c r="B12" s="31" t="s">
         <v>150</v>
       </c>

</xml_diff>